<commit_message>
migration bug fix, add’l data
</commit_message>
<xml_diff>
--- a/data/paradox/2019-01-18-Titans-Legacy.xlsx
+++ b/data/paradox/2019-01-18-Titans-Legacy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjessup/Documents/Development/PublicSource/clash-stats/data/paradox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F13A6B-6C37-1C46-A6FD-839D897C8FDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF60F40-80CE-EE44-AFD5-40A6600F271E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59460" yWindow="3640" windowWidth="20920" windowHeight="22180" xr2:uid="{57268BF6-2F68-1E40-9496-9B9C88D25D1B}"/>
+    <workbookView xWindow="1760" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{57268BF6-2F68-1E40-9496-9B9C88D25D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -395,6 +395,30 @@
           </cell>
           <cell r="B26" t="str">
             <v>LQCVQJ9G</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>G Squad</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>JJPVG0GJ</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>Delivering Chaos</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>YRVGGUG8</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>g-solo</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>QR9PU9CU</v>
           </cell>
         </row>
       </sheetData>
@@ -703,7 +727,7 @@
   <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>